<commit_message>
Updated main.py and colormaps
Added more custom colormaps and documentation
</commit_message>
<xml_diff>
--- a/resources/app_data/custom_colormaps.xlsx
+++ b/resources/app_data/custom_colormaps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhasterok/Documents/GitHub/LaserMapExplorer/resources/app_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derrickhasterok/GitHub/LaserMapExplorer/resources/app_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AEF7CE-1365-8A48-8269-AF295005063D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4081E4FA-CFD8-F14D-933C-507857952FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30600" yWindow="9940" windowWidth="19400" windowHeight="17440" xr2:uid="{D6A79B19-0972-6E47-B8F8-44D0860CB5DE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34860" windowHeight="21900" xr2:uid="{D6A79B19-0972-6E47-B8F8-44D0860CB5DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="297">
   <si>
     <t>#191D26</t>
   </si>
@@ -209,9 +209,6 @@
     <t>#281319</t>
   </si>
   <si>
-    <t>#1C0B0C</t>
-  </si>
-  <si>
     <t>#4D1C12</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>#84CA99</t>
   </si>
   <si>
-    <t>#A9D48D</t>
-  </si>
-  <si>
     <t>#65BC4A</t>
   </si>
   <si>
@@ -473,9 +467,6 @@
     <t>#060609</t>
   </si>
   <si>
-    <t>#0A2523</t>
-  </si>
-  <si>
     <t>#053027</t>
   </si>
   <si>
@@ -687,6 +678,255 @@
   </si>
   <si>
     <t>#F0F921</t>
+  </si>
+  <si>
+    <t>#D92E27</t>
+  </si>
+  <si>
+    <t>#96CC6F</t>
+  </si>
+  <si>
+    <t>#AAAD9C</t>
+  </si>
+  <si>
+    <t>lake eyre</t>
+  </si>
+  <si>
+    <t>#896c5e</t>
+  </si>
+  <si>
+    <t>#6e7844</t>
+  </si>
+  <si>
+    <t>#a29d4e</t>
+  </si>
+  <si>
+    <t>#da8427</t>
+  </si>
+  <si>
+    <t>#cd953b</t>
+  </si>
+  <si>
+    <t>#b44e26</t>
+  </si>
+  <si>
+    <t>#a13835</t>
+  </si>
+  <si>
+    <t>#d3899a</t>
+  </si>
+  <si>
+    <t>#daa5a2</t>
+  </si>
+  <si>
+    <t>sunspot</t>
+  </si>
+  <si>
+    <t>#1a0f10</t>
+  </si>
+  <si>
+    <t>#812f19</t>
+  </si>
+  <si>
+    <t>#ab4825</t>
+  </si>
+  <si>
+    <t>#d26b28</t>
+  </si>
+  <si>
+    <t>#dc7c27</t>
+  </si>
+  <si>
+    <t>#f1ae4b</t>
+  </si>
+  <si>
+    <t>#fee28a</t>
+  </si>
+  <si>
+    <t>#fff9ce</t>
+  </si>
+  <si>
+    <t>wheatfield</t>
+  </si>
+  <si>
+    <t>#652f12</t>
+  </si>
+  <si>
+    <t>#953a1f</t>
+  </si>
+  <si>
+    <t>#ce6728</t>
+  </si>
+  <si>
+    <t>#e49b33</t>
+  </si>
+  <si>
+    <t>#fec553</t>
+  </si>
+  <si>
+    <t>#f0d047</t>
+  </si>
+  <si>
+    <t>#f9dea9</t>
+  </si>
+  <si>
+    <t>#fff6d7</t>
+  </si>
+  <si>
+    <t>#efeee9</t>
+  </si>
+  <si>
+    <t>#d8e8f2</t>
+  </si>
+  <si>
+    <t>#b6d6e9</t>
+  </si>
+  <si>
+    <t>#96cce5</t>
+  </si>
+  <si>
+    <t>#76b0d0</t>
+  </si>
+  <si>
+    <t>red chilli</t>
+  </si>
+  <si>
+    <t>#140a0a</t>
+  </si>
+  <si>
+    <t>#721011</t>
+  </si>
+  <si>
+    <t>#8c181b</t>
+  </si>
+  <si>
+    <t>#c32026</t>
+  </si>
+  <si>
+    <t>#ef556b</t>
+  </si>
+  <si>
+    <t>#f27997</t>
+  </si>
+  <si>
+    <t>#f8bfd8</t>
+  </si>
+  <si>
+    <t>#eddfe7</t>
+  </si>
+  <si>
+    <t>citrus</t>
+  </si>
+  <si>
+    <t>#3b1122</t>
+  </si>
+  <si>
+    <t>#620a1a</t>
+  </si>
+  <si>
+    <t>#eb4c70</t>
+  </si>
+  <si>
+    <t>#f57f20</t>
+  </si>
+  <si>
+    <t>#f89a1c</t>
+  </si>
+  <si>
+    <t>#fecf0c</t>
+  </si>
+  <si>
+    <t>#fced0e</t>
+  </si>
+  <si>
+    <t>#9cc447</t>
+  </si>
+  <si>
+    <t>#68bd47</t>
+  </si>
+  <si>
+    <t>#3d793a</t>
+  </si>
+  <si>
+    <t>golden wattle</t>
+  </si>
+  <si>
+    <t>#263522</t>
+  </si>
+  <si>
+    <t>#59725c</t>
+  </si>
+  <si>
+    <t>#819491</t>
+  </si>
+  <si>
+    <t>#91aaa4</t>
+  </si>
+  <si>
+    <t>#ba92ac</t>
+  </si>
+  <si>
+    <t>#af6834</t>
+  </si>
+  <si>
+    <t>#b18e2f</t>
+  </si>
+  <si>
+    <t>#dfa826</t>
+  </si>
+  <si>
+    <t>#e6c220</t>
+  </si>
+  <si>
+    <t>#feeb2c</t>
+  </si>
+  <si>
+    <t>#C22E27</t>
+  </si>
+  <si>
+    <t>watermelon tourmaline</t>
+  </si>
+  <si>
+    <t>#152313</t>
+  </si>
+  <si>
+    <t>#466c40</t>
+  </si>
+  <si>
+    <t>#79bb79</t>
+  </si>
+  <si>
+    <t>#c5e1af</t>
+  </si>
+  <si>
+    <t>#f9f7fb</t>
+  </si>
+  <si>
+    <t>#e59bc4</t>
+  </si>
+  <si>
+    <t>#e763a5</t>
+  </si>
+  <si>
+    <t>#a61d4e</t>
+  </si>
+  <si>
+    <t>#43111b</t>
+  </si>
+  <si>
+    <t>#6097be</t>
+  </si>
+  <si>
+    <t>#3d83af</t>
+  </si>
+  <si>
+    <t>#156499</t>
+  </si>
+  <si>
+    <t>#DBDBD9</t>
+  </si>
+  <si>
+    <t>#EFEFFF</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02F9D18-E15D-7543-BDDB-CEAF3D6E755C}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,9 +1309,9 @@
     <col min="1" max="1" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1116,9 +1356,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1163,9 +1403,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -1210,9 +1450,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -1257,567 +1497,821 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="M5" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="N5" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="O5" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="P5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="L6" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="N6" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="O6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="s">
         <v>84</v>
       </c>
-      <c r="P6" t="s">
+      <c r="C7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>87</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>88</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>89</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>90</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>91</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>92</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>93</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>94</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>95</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>96</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>97</v>
       </c>
-      <c r="N7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="K8" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="L8" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="M8" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="N8" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="O8" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="P8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F9" t="s">
+        <v>241</v>
+      </c>
+      <c r="G9" t="s">
+        <v>242</v>
+      </c>
+      <c r="H9" t="s">
+        <v>243</v>
+      </c>
+      <c r="I9" t="s">
+        <v>244</v>
+      </c>
+      <c r="J9" t="s">
+        <v>245</v>
+      </c>
+      <c r="K9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L9" t="s">
+        <v>247</v>
+      </c>
+      <c r="M9" t="s">
+        <v>248</v>
+      </c>
+      <c r="N9" t="s">
+        <v>249</v>
+      </c>
+      <c r="O9" t="s">
+        <v>292</v>
+      </c>
+      <c r="P9" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" t="s">
+        <v>285</v>
+      </c>
+      <c r="E10" t="s">
+        <v>286</v>
+      </c>
+      <c r="F10" t="s">
+        <v>287</v>
+      </c>
+      <c r="G10" t="s">
+        <v>288</v>
+      </c>
+      <c r="H10" t="s">
+        <v>289</v>
+      </c>
+      <c r="I10" t="s">
+        <v>290</v>
+      </c>
+      <c r="J10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>170</v>
       </c>
-      <c r="B9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G9" t="s">
-        <v>120</v>
-      </c>
-      <c r="H9" t="s">
-        <v>121</v>
-      </c>
-      <c r="I9" t="s">
-        <v>122</v>
-      </c>
-      <c r="J9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K9" t="s">
-        <v>124</v>
-      </c>
-      <c r="L9" t="s">
-        <v>125</v>
-      </c>
-      <c r="M9" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" t="s">
-        <v>127</v>
-      </c>
-      <c r="O9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" t="s">
-        <v>133</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L11" t="s">
+        <v>215</v>
+      </c>
+      <c r="M11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" t="s">
+        <v>82</v>
+      </c>
+      <c r="P11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" t="s">
         <v>134</v>
       </c>
-      <c r="I10" t="s">
+      <c r="C12" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D12" t="s">
         <v>136</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E12" t="s">
         <v>137</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F12" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" t="s">
         <v>138</v>
       </c>
-      <c r="E11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="H12" t="s">
+        <v>140</v>
+      </c>
+      <c r="I12" t="s">
         <v>141</v>
       </c>
-      <c r="G11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11" t="s">
-        <v>142</v>
-      </c>
-      <c r="I11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G12" t="s">
-        <v>149</v>
-      </c>
-      <c r="H12" t="s">
-        <v>150</v>
-      </c>
-      <c r="I12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>166</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="F13" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="G13" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="H13" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="I13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="J13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>187</v>
+        <v>144</v>
       </c>
       <c r="E14" t="s">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="F14" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="G14" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="H14" t="s">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="I14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="J14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>227</v>
       </c>
       <c r="B15" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="C15" t="s">
-        <v>190</v>
+        <v>229</v>
       </c>
       <c r="D15" t="s">
-        <v>191</v>
+        <v>230</v>
       </c>
       <c r="E15" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="F15" t="s">
-        <v>188</v>
+        <v>232</v>
       </c>
       <c r="G15" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
       <c r="H15" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="I15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="D16" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="E16" t="s">
+        <v>214</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" t="s">
+        <v>153</v>
+      </c>
+      <c r="H16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I16" t="s">
+        <v>155</v>
+      </c>
+      <c r="J16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" t="s">
+        <v>253</v>
+      </c>
+      <c r="E17" t="s">
+        <v>254</v>
+      </c>
+      <c r="F17" t="s">
+        <v>255</v>
+      </c>
+      <c r="G17" t="s">
+        <v>256</v>
+      </c>
+      <c r="H17" t="s">
+        <v>257</v>
+      </c>
+      <c r="I17" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" t="s">
         <v>182</v>
       </c>
-      <c r="F16" t="s">
-        <v>193</v>
-      </c>
-      <c r="G16" t="s">
-        <v>194</v>
-      </c>
-      <c r="H16" t="s">
-        <v>195</v>
-      </c>
-      <c r="I16" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>162</v>
-      </c>
-      <c r="B17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>183</v>
       </c>
-      <c r="D17" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" t="s">
-        <v>198</v>
-      </c>
-      <c r="F17" t="s">
-        <v>199</v>
-      </c>
-      <c r="G17" t="s">
-        <v>200</v>
-      </c>
-      <c r="H17" t="s">
-        <v>201</v>
-      </c>
-      <c r="I17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>160</v>
-      </c>
-      <c r="B18" t="s">
-        <v>202</v>
-      </c>
-      <c r="C18" t="s">
-        <v>203</v>
-      </c>
       <c r="D18" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="E18" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="F18" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="G18" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="H18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>161</v>
       </c>
       <c r="B19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G19" t="s">
+        <v>185</v>
+      </c>
+      <c r="H19" t="s">
+        <v>185</v>
+      </c>
+      <c r="I19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" t="s">
+        <v>191</v>
+      </c>
+      <c r="H20" t="s">
+        <v>192</v>
+      </c>
+      <c r="I20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F21" t="s">
+        <v>196</v>
+      </c>
+      <c r="G21" t="s">
+        <v>197</v>
+      </c>
+      <c r="H21" t="s">
+        <v>198</v>
+      </c>
+      <c r="I21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D22" t="s">
+        <v>201</v>
+      </c>
+      <c r="E22" t="s">
+        <v>202</v>
+      </c>
+      <c r="F22" t="s">
+        <v>203</v>
+      </c>
+      <c r="G22" t="s">
+        <v>204</v>
+      </c>
+      <c r="H22" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23" t="s">
+        <v>202</v>
+      </c>
+      <c r="F23" t="s">
+        <v>203</v>
+      </c>
+      <c r="G23" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" t="s">
+        <v>185</v>
+      </c>
+      <c r="I23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" t="s">
         <v>208</v>
       </c>
-      <c r="C19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D19" t="s">
-        <v>184</v>
-      </c>
-      <c r="E19" t="s">
-        <v>205</v>
-      </c>
-      <c r="F19" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H19" t="s">
-        <v>188</v>
-      </c>
-      <c r="I19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="E24" t="s">
         <v>209</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F24" t="s">
         <v>210</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G24" t="s">
         <v>211</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H24" t="s">
         <v>212</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I24" t="s">
         <v>213</v>
       </c>
-      <c r="G20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H20" t="s">
-        <v>215</v>
-      </c>
-      <c r="I20" t="s">
-        <v>216</v>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>217</v>
+      </c>
+      <c r="B25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" t="s">
+        <v>222</v>
+      </c>
+      <c r="G25" t="s">
+        <v>223</v>
+      </c>
+      <c r="H25" t="s">
+        <v>224</v>
+      </c>
+      <c r="I25" t="s">
+        <v>225</v>
+      </c>
+      <c r="J25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>259</v>
+      </c>
+      <c r="B26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D26" t="s">
+        <v>262</v>
+      </c>
+      <c r="E26" t="s">
+        <v>263</v>
+      </c>
+      <c r="F26" t="s">
+        <v>264</v>
+      </c>
+      <c r="G26" t="s">
+        <v>265</v>
+      </c>
+      <c r="H26" t="s">
+        <v>266</v>
+      </c>
+      <c r="I26" t="s">
+        <v>267</v>
+      </c>
+      <c r="J26" t="s">
+        <v>268</v>
+      </c>
+      <c r="K26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" t="s">
+        <v>271</v>
+      </c>
+      <c r="C27" t="s">
+        <v>272</v>
+      </c>
+      <c r="D27" t="s">
+        <v>273</v>
+      </c>
+      <c r="E27" t="s">
+        <v>274</v>
+      </c>
+      <c r="F27" t="s">
+        <v>275</v>
+      </c>
+      <c r="G27" t="s">
+        <v>276</v>
+      </c>
+      <c r="H27" t="s">
+        <v>277</v>
+      </c>
+      <c r="I27" t="s">
+        <v>278</v>
+      </c>
+      <c r="J27" t="s">
+        <v>279</v>
+      </c>
+      <c r="K27" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>